<commit_message>
Yooo my guy we got to style now leeetttss goood ok and yeah actually add the optional vals
Today we did some error correction and we where happy that is works now kind of

Yoo listen fam you keep it going u got this and remember brush your teeth and no bed until your done big ups have a nice day today or tomorrow yeah
</commit_message>
<xml_diff>
--- a/src/main/resources/Excel-Files/Static_Content.xlsx
+++ b/src/main/resources/Excel-Files/Static_Content.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lkronlac\Desktop\Data\Project\TemplateCreator\TemplateCreator\src\main\resources\Excel-Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lkronlac\Desktop\Data\Project\Frontend\CreatorFrontend\Frontend\src\main\resources\Excel-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683CBDE1-0168-4BCB-9508-F5708E93D381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC57954-21E8-4F5A-9476-168E877DB92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{58DF28F6-9EB8-486E-99A6-F7AC2F9EA8FC}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{58DF28F6-9EB8-486E-99A6-F7AC2F9EA8FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover + TOC" sheetId="2" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="236">
   <si>
     <t>Daily Rates (8 hours):</t>
   </si>
@@ -1828,6 +1828,9 @@
       </rPr>
       <t>approx. &lt;000.000&gt; master data address records, approx. &lt;000.000&gt; BOMs with approx. &lt;000.000&gt; parts for which approx. &lt;00.000&gt; LTSDs are requested annually.</t>
     </r>
+  </si>
+  <si>
+    <t>&lt;Maintenance&gt;%</t>
   </si>
 </sst>
 </file>
@@ -2531,15 +2534,45 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2576,36 +2609,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2629,28 +2632,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -2664,10 +2645,41 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
@@ -2676,15 +2688,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2781,8 +2784,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="22861" y="1082712"/>
-          <a:ext cx="5888579" cy="4745690"/>
+          <a:off x="19051" y="1139862"/>
+          <a:ext cx="5894294" cy="4991435"/>
           <a:chOff x="0" y="1247775"/>
           <a:chExt cx="5924550" cy="4734709"/>
         </a:xfrm>
@@ -4342,47 +4345,47 @@
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="88.7109375" style="19" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="19" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="19"/>
+    <col min="1" max="1" width="88.6640625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="19" customWidth="1"/>
+    <col min="3" max="16384" width="11.44140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
     </row>
-    <row r="33" spans="1:1" ht="33" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" ht="32.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="23"/>
     </row>
-    <row r="36" spans="1:1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" ht="44.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="22" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" ht="25.2" x14ac:dyDescent="0.45">
       <c r="A37" s="22"/>
     </row>
-    <row r="38" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:1" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A39" s="21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="101" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:1" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A46" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -4400,42 +4403,42 @@
   </sheetPr>
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.7109375" customWidth="1"/>
+    <col min="1" max="1" width="66.6640625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="4" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
     <col min="7" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" customWidth="1"/>
-    <col min="12" max="14" width="16.140625" customWidth="1"/>
-    <col min="15" max="30" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="14" width="16.109375" customWidth="1"/>
+    <col min="15" max="30" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="152" t="s">
+    <row r="1" spans="1:14" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="137" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
-      <c r="H1" s="152"/>
-      <c r="I1" s="152"/>
-      <c r="J1" s="152"/>
-      <c r="K1" s="152"/>
-      <c r="L1" s="152"/>
-      <c r="M1" s="152"/>
-      <c r="N1" s="152"/>
-    </row>
-    <row r="2" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
+      <c r="J1" s="137"/>
+      <c r="K1" s="137"/>
+      <c r="L1" s="137"/>
+      <c r="M1" s="137"/>
+      <c r="N1" s="137"/>
+    </row>
+    <row r="2" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4451,7 +4454,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>231</v>
       </c>
@@ -4469,7 +4472,7 @@
       <c r="M3" s="4"/>
       <c r="N3" s="5"/>
     </row>
-    <row r="4" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -4485,7 +4488,7 @@
       <c r="M4" s="7"/>
       <c r="N4" s="8"/>
     </row>
-    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="100" t="s">
         <v>230</v>
       </c>
@@ -4503,7 +4506,7 @@
       <c r="M5" s="7"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="100" t="s">
         <v>232</v>
       </c>
@@ -4521,7 +4524,7 @@
       <c r="M6" s="9"/>
       <c r="N6" s="8"/>
     </row>
-    <row r="7" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="10"/>
       <c r="C7" s="7"/>
@@ -4537,7 +4540,7 @@
       <c r="M7" s="7"/>
       <c r="N7" s="8"/>
     </row>
-    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>0</v>
       </c>
@@ -4555,7 +4558,7 @@
       <c r="M8" s="7"/>
       <c r="N8" s="8"/>
     </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>1</v>
       </c>
@@ -4577,7 +4580,7 @@
       <c r="M9" s="12"/>
       <c r="N9" s="8"/>
     </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>3</v>
       </c>
@@ -4599,7 +4602,7 @@
       <c r="M10" s="12"/>
       <c r="N10" s="8"/>
     </row>
-    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>4</v>
       </c>
@@ -4621,7 +4624,7 @@
       <c r="M11" s="12"/>
       <c r="N11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>5</v>
       </c>
@@ -4643,7 +4646,7 @@
       <c r="M12" s="12"/>
       <c r="N12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="13"/>
       <c r="C13" s="7"/>
@@ -4659,29 +4662,29 @@
       <c r="M13" s="7"/>
       <c r="N13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="15">
-        <v>0.18</v>
-      </c>
-      <c r="C14" s="135" t="s">
+      <c r="B14" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="C14" s="138" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="135"/>
-      <c r="E14" s="135"/>
-      <c r="F14" s="135"/>
-      <c r="G14" s="135"/>
-      <c r="H14" s="135"/>
-      <c r="I14" s="135"/>
-      <c r="J14" s="135"/>
-      <c r="K14" s="135"/>
-      <c r="L14" s="135"/>
-      <c r="M14" s="135"/>
-      <c r="N14" s="136"/>
-    </row>
-    <row r="15" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="138"/>
+      <c r="E14" s="138"/>
+      <c r="F14" s="138"/>
+      <c r="G14" s="138"/>
+      <c r="H14" s="138"/>
+      <c r="I14" s="138"/>
+      <c r="J14" s="138"/>
+      <c r="K14" s="138"/>
+      <c r="L14" s="138"/>
+      <c r="M14" s="138"/>
+      <c r="N14" s="139"/>
+    </row>
+    <row r="15" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="13"/>
       <c r="C15" s="7"/>
@@ -4697,223 +4700,223 @@
       <c r="M15" s="7"/>
       <c r="N15" s="8"/>
     </row>
-    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="153" t="s">
+    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="140" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
-      <c r="M16" s="154"/>
-      <c r="N16" s="155"/>
-    </row>
-    <row r="17" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="156" t="s">
+      <c r="B16" s="141"/>
+      <c r="C16" s="141"/>
+      <c r="D16" s="141"/>
+      <c r="E16" s="141"/>
+      <c r="F16" s="141"/>
+      <c r="G16" s="141"/>
+      <c r="H16" s="141"/>
+      <c r="I16" s="141"/>
+      <c r="J16" s="141"/>
+      <c r="K16" s="141"/>
+      <c r="L16" s="141"/>
+      <c r="M16" s="141"/>
+      <c r="N16" s="142"/>
+    </row>
+    <row r="17" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="143" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="157"/>
-      <c r="C17" s="157"/>
-      <c r="D17" s="157"/>
-      <c r="E17" s="157"/>
-      <c r="F17" s="157"/>
-      <c r="G17" s="157"/>
-      <c r="H17" s="157"/>
-      <c r="I17" s="157"/>
-      <c r="J17" s="157"/>
-      <c r="K17" s="157"/>
-      <c r="L17" s="157"/>
-      <c r="M17" s="157"/>
-      <c r="N17" s="158"/>
-    </row>
-    <row r="18" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="134" t="s">
+      <c r="B17" s="144"/>
+      <c r="C17" s="144"/>
+      <c r="D17" s="144"/>
+      <c r="E17" s="144"/>
+      <c r="F17" s="144"/>
+      <c r="G17" s="144"/>
+      <c r="H17" s="144"/>
+      <c r="I17" s="144"/>
+      <c r="J17" s="144"/>
+      <c r="K17" s="144"/>
+      <c r="L17" s="144"/>
+      <c r="M17" s="144"/>
+      <c r="N17" s="145"/>
+    </row>
+    <row r="18" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="146" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="135"/>
-      <c r="C18" s="135"/>
-      <c r="D18" s="135"/>
-      <c r="E18" s="135"/>
-      <c r="F18" s="135"/>
-      <c r="G18" s="135"/>
-      <c r="H18" s="135"/>
-      <c r="I18" s="135"/>
-      <c r="J18" s="135"/>
-      <c r="K18" s="135"/>
-      <c r="L18" s="135"/>
-      <c r="M18" s="135"/>
-      <c r="N18" s="136"/>
-    </row>
-    <row r="19" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="149" t="s">
+      <c r="B18" s="138"/>
+      <c r="C18" s="138"/>
+      <c r="D18" s="138"/>
+      <c r="E18" s="138"/>
+      <c r="F18" s="138"/>
+      <c r="G18" s="138"/>
+      <c r="H18" s="138"/>
+      <c r="I18" s="138"/>
+      <c r="J18" s="138"/>
+      <c r="K18" s="138"/>
+      <c r="L18" s="138"/>
+      <c r="M18" s="138"/>
+      <c r="N18" s="139"/>
+    </row>
+    <row r="19" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="134" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="150"/>
-      <c r="C19" s="150"/>
-      <c r="D19" s="150"/>
-      <c r="E19" s="150"/>
-      <c r="F19" s="150"/>
-      <c r="G19" s="150"/>
-      <c r="H19" s="150"/>
-      <c r="I19" s="150"/>
-      <c r="J19" s="150"/>
-      <c r="K19" s="150"/>
-      <c r="L19" s="150"/>
-      <c r="M19" s="150"/>
-      <c r="N19" s="151"/>
-    </row>
-    <row r="20" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="140" t="s">
+      <c r="B19" s="135"/>
+      <c r="C19" s="135"/>
+      <c r="D19" s="135"/>
+      <c r="E19" s="135"/>
+      <c r="F19" s="135"/>
+      <c r="G19" s="135"/>
+      <c r="H19" s="135"/>
+      <c r="I19" s="135"/>
+      <c r="J19" s="135"/>
+      <c r="K19" s="135"/>
+      <c r="L19" s="135"/>
+      <c r="M19" s="135"/>
+      <c r="N19" s="136"/>
+    </row>
+    <row r="20" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="141"/>
-      <c r="C20" s="141"/>
-      <c r="D20" s="141"/>
-      <c r="E20" s="141"/>
-      <c r="F20" s="141"/>
-      <c r="G20" s="141"/>
-      <c r="H20" s="141"/>
-      <c r="I20" s="141"/>
-      <c r="J20" s="141"/>
-      <c r="K20" s="141"/>
-      <c r="L20" s="141"/>
-      <c r="M20" s="141"/>
-      <c r="N20" s="142"/>
-    </row>
-    <row r="21" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="143" t="s">
+      <c r="B20" s="151"/>
+      <c r="C20" s="151"/>
+      <c r="D20" s="151"/>
+      <c r="E20" s="151"/>
+      <c r="F20" s="151"/>
+      <c r="G20" s="151"/>
+      <c r="H20" s="151"/>
+      <c r="I20" s="151"/>
+      <c r="J20" s="151"/>
+      <c r="K20" s="151"/>
+      <c r="L20" s="151"/>
+      <c r="M20" s="151"/>
+      <c r="N20" s="152"/>
+    </row>
+    <row r="21" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="153" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="144"/>
-      <c r="C21" s="144"/>
-      <c r="D21" s="144"/>
-      <c r="E21" s="144"/>
-      <c r="F21" s="144"/>
-      <c r="G21" s="144"/>
-      <c r="H21" s="144"/>
-      <c r="I21" s="144"/>
-      <c r="J21" s="144"/>
-      <c r="K21" s="144"/>
-      <c r="L21" s="144"/>
-      <c r="M21" s="144"/>
-      <c r="N21" s="145"/>
-    </row>
-    <row r="22" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="140" t="s">
+      <c r="B21" s="154"/>
+      <c r="C21" s="154"/>
+      <c r="D21" s="154"/>
+      <c r="E21" s="154"/>
+      <c r="F21" s="154"/>
+      <c r="G21" s="154"/>
+      <c r="H21" s="154"/>
+      <c r="I21" s="154"/>
+      <c r="J21" s="154"/>
+      <c r="K21" s="154"/>
+      <c r="L21" s="154"/>
+      <c r="M21" s="154"/>
+      <c r="N21" s="155"/>
+    </row>
+    <row r="22" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="150" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="141"/>
-      <c r="C22" s="141"/>
-      <c r="D22" s="141"/>
-      <c r="E22" s="141"/>
-      <c r="F22" s="141"/>
-      <c r="G22" s="141"/>
-      <c r="H22" s="141"/>
-      <c r="I22" s="141"/>
-      <c r="J22" s="141"/>
-      <c r="K22" s="141"/>
-      <c r="L22" s="141"/>
-      <c r="M22" s="141"/>
-      <c r="N22" s="142"/>
-    </row>
-    <row r="23" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="143" t="s">
+      <c r="B22" s="151"/>
+      <c r="C22" s="151"/>
+      <c r="D22" s="151"/>
+      <c r="E22" s="151"/>
+      <c r="F22" s="151"/>
+      <c r="G22" s="151"/>
+      <c r="H22" s="151"/>
+      <c r="I22" s="151"/>
+      <c r="J22" s="151"/>
+      <c r="K22" s="151"/>
+      <c r="L22" s="151"/>
+      <c r="M22" s="151"/>
+      <c r="N22" s="152"/>
+    </row>
+    <row r="23" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="153" t="s">
         <v>233</v>
       </c>
-      <c r="B23" s="144"/>
-      <c r="C23" s="144"/>
-      <c r="D23" s="144"/>
-      <c r="E23" s="144"/>
-      <c r="F23" s="144"/>
-      <c r="G23" s="144"/>
-      <c r="H23" s="144"/>
-      <c r="I23" s="144"/>
-      <c r="J23" s="144"/>
-      <c r="K23" s="144"/>
-      <c r="L23" s="144"/>
-      <c r="M23" s="144"/>
-      <c r="N23" s="145"/>
-    </row>
-    <row r="24" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="146" t="s">
+      <c r="B23" s="154"/>
+      <c r="C23" s="154"/>
+      <c r="D23" s="154"/>
+      <c r="E23" s="154"/>
+      <c r="F23" s="154"/>
+      <c r="G23" s="154"/>
+      <c r="H23" s="154"/>
+      <c r="I23" s="154"/>
+      <c r="J23" s="154"/>
+      <c r="K23" s="154"/>
+      <c r="L23" s="154"/>
+      <c r="M23" s="154"/>
+      <c r="N23" s="155"/>
+    </row>
+    <row r="24" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="156" t="s">
         <v>234</v>
       </c>
-      <c r="B24" s="147"/>
-      <c r="C24" s="147"/>
-      <c r="D24" s="147"/>
-      <c r="E24" s="147"/>
-      <c r="F24" s="147"/>
-      <c r="G24" s="147"/>
-      <c r="H24" s="147"/>
-      <c r="I24" s="147"/>
-      <c r="J24" s="147"/>
-      <c r="K24" s="147"/>
-      <c r="L24" s="147"/>
-      <c r="M24" s="147"/>
-      <c r="N24" s="148"/>
-    </row>
-    <row r="25" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="149" t="s">
+      <c r="B24" s="157"/>
+      <c r="C24" s="157"/>
+      <c r="D24" s="157"/>
+      <c r="E24" s="157"/>
+      <c r="F24" s="157"/>
+      <c r="G24" s="157"/>
+      <c r="H24" s="157"/>
+      <c r="I24" s="157"/>
+      <c r="J24" s="157"/>
+      <c r="K24" s="157"/>
+      <c r="L24" s="157"/>
+      <c r="M24" s="157"/>
+      <c r="N24" s="158"/>
+    </row>
+    <row r="25" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="134" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="150"/>
-      <c r="C25" s="150"/>
-      <c r="D25" s="150"/>
-      <c r="E25" s="150"/>
-      <c r="F25" s="150"/>
-      <c r="G25" s="150"/>
-      <c r="H25" s="150"/>
-      <c r="I25" s="150"/>
-      <c r="J25" s="150"/>
-      <c r="K25" s="150"/>
-      <c r="L25" s="150"/>
-      <c r="M25" s="150"/>
-      <c r="N25" s="151"/>
-    </row>
-    <row r="26" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="134" t="s">
+      <c r="B25" s="135"/>
+      <c r="C25" s="135"/>
+      <c r="D25" s="135"/>
+      <c r="E25" s="135"/>
+      <c r="F25" s="135"/>
+      <c r="G25" s="135"/>
+      <c r="H25" s="135"/>
+      <c r="I25" s="135"/>
+      <c r="J25" s="135"/>
+      <c r="K25" s="135"/>
+      <c r="L25" s="135"/>
+      <c r="M25" s="135"/>
+      <c r="N25" s="136"/>
+    </row>
+    <row r="26" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="146" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="135"/>
-      <c r="C26" s="135"/>
-      <c r="D26" s="135"/>
-      <c r="E26" s="135"/>
-      <c r="F26" s="135"/>
-      <c r="G26" s="135"/>
-      <c r="H26" s="135"/>
-      <c r="I26" s="135"/>
-      <c r="J26" s="135"/>
-      <c r="K26" s="135"/>
-      <c r="L26" s="135"/>
-      <c r="M26" s="135"/>
-      <c r="N26" s="136"/>
-    </row>
-    <row r="27" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="137" t="s">
+      <c r="B26" s="138"/>
+      <c r="C26" s="138"/>
+      <c r="D26" s="138"/>
+      <c r="E26" s="138"/>
+      <c r="F26" s="138"/>
+      <c r="G26" s="138"/>
+      <c r="H26" s="138"/>
+      <c r="I26" s="138"/>
+      <c r="J26" s="138"/>
+      <c r="K26" s="138"/>
+      <c r="L26" s="138"/>
+      <c r="M26" s="138"/>
+      <c r="N26" s="139"/>
+    </row>
+    <row r="27" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="147" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="138"/>
-      <c r="C27" s="138"/>
-      <c r="D27" s="138"/>
-      <c r="E27" s="138"/>
-      <c r="F27" s="138"/>
-      <c r="G27" s="138"/>
-      <c r="H27" s="138"/>
-      <c r="I27" s="138"/>
-      <c r="J27" s="138"/>
-      <c r="K27" s="138"/>
-      <c r="L27" s="138"/>
-      <c r="M27" s="138"/>
-      <c r="N27" s="139"/>
-    </row>
-    <row r="28" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="148"/>
+      <c r="C27" s="148"/>
+      <c r="D27" s="148"/>
+      <c r="E27" s="148"/>
+      <c r="F27" s="148"/>
+      <c r="G27" s="148"/>
+      <c r="H27" s="148"/>
+      <c r="I27" s="148"/>
+      <c r="J27" s="148"/>
+      <c r="K27" s="148"/>
+      <c r="L27" s="148"/>
+      <c r="M27" s="148"/>
+      <c r="N27" s="149"/>
+    </row>
+    <row r="28" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
@@ -4929,15 +4932,9 @@
       <c r="M28" s="17"/>
       <c r="N28" s="18"/>
     </row>
-    <row r="29" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A19:N19"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="C14:N14"/>
-    <mergeCell ref="A16:N16"/>
-    <mergeCell ref="A17:N17"/>
-    <mergeCell ref="A18:N18"/>
     <mergeCell ref="A26:N26"/>
     <mergeCell ref="A27:N27"/>
     <mergeCell ref="A20:N20"/>
@@ -4946,6 +4943,12 @@
     <mergeCell ref="A23:N23"/>
     <mergeCell ref="A24:N24"/>
     <mergeCell ref="A25:N25"/>
+    <mergeCell ref="A19:N19"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="C14:N14"/>
+    <mergeCell ref="A16:N16"/>
+    <mergeCell ref="A17:N17"/>
+    <mergeCell ref="A18:N18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4965,19 +4968,19 @@
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="19" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" style="19" customWidth="1"/>
-    <col min="3" max="3" width="3.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="19" customWidth="1"/>
-    <col min="5" max="5" width="53.28515625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="43.85546875" style="19" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="19" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="19"/>
+    <col min="2" max="2" width="4.88671875" style="19" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="53.33203125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="43.88671875" style="19" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="19" customWidth="1"/>
+    <col min="8" max="16384" width="11.44140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="159" t="s">
         <v>67</v>
       </c>
@@ -4987,7 +4990,7 @@
       <c r="F3" s="160"/>
       <c r="G3" s="160"/>
     </row>
-    <row r="5" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" s="25" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A5" s="42"/>
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
@@ -4996,7 +4999,7 @@
       <c r="F5" s="41"/>
       <c r="G5" s="40"/>
     </row>
-    <row r="6" spans="1:20" s="25" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" s="25" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="35"/>
       <c r="B6" s="161" t="s">
         <v>66</v>
@@ -5019,7 +5022,7 @@
       <c r="S6" s="29"/>
       <c r="T6" s="29"/>
     </row>
-    <row r="7" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="35"/>
       <c r="B7" s="34" t="s">
         <v>65</v>
@@ -5042,7 +5045,7 @@
       <c r="S7" s="29"/>
       <c r="T7" s="29"/>
     </row>
-    <row r="8" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="35"/>
       <c r="B8" s="34" t="s">
         <v>64</v>
@@ -5065,7 +5068,7 @@
       <c r="S8" s="29"/>
       <c r="T8" s="29"/>
     </row>
-    <row r="9" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="35"/>
       <c r="B9" s="34"/>
       <c r="C9" s="36"/>
@@ -5086,7 +5089,7 @@
       <c r="S9" s="29"/>
       <c r="T9" s="29"/>
     </row>
-    <row r="10" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="35"/>
       <c r="B10" s="38" t="s">
         <v>63</v>
@@ -5109,7 +5112,7 @@
       <c r="S10" s="29"/>
       <c r="T10" s="29"/>
     </row>
-    <row r="11" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="35"/>
       <c r="B11" s="34" t="s">
         <v>62</v>
@@ -5132,7 +5135,7 @@
       <c r="S11" s="29"/>
       <c r="T11" s="29"/>
     </row>
-    <row r="12" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="35"/>
       <c r="B12" s="34" t="s">
         <v>61</v>
@@ -5155,7 +5158,7 @@
       <c r="S12" s="29"/>
       <c r="T12" s="29"/>
     </row>
-    <row r="13" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="35"/>
       <c r="B13" s="34" t="s">
         <v>60</v>
@@ -5178,7 +5181,7 @@
       <c r="S13" s="29"/>
       <c r="T13" s="29"/>
     </row>
-    <row r="14" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="35"/>
       <c r="B14" s="34" t="s">
         <v>59</v>
@@ -5201,7 +5204,7 @@
       <c r="S14" s="29"/>
       <c r="T14" s="29"/>
     </row>
-    <row r="15" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="35"/>
       <c r="B15" s="34" t="s">
         <v>58</v>
@@ -5224,7 +5227,7 @@
       <c r="S15" s="29"/>
       <c r="T15" s="29"/>
     </row>
-    <row r="16" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="35"/>
       <c r="B16" s="34" t="s">
         <v>57</v>
@@ -5247,7 +5250,7 @@
       <c r="S16" s="29"/>
       <c r="T16" s="29"/>
     </row>
-    <row r="17" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="35"/>
       <c r="B17" s="34" t="s">
         <v>56</v>
@@ -5270,7 +5273,7 @@
       <c r="S17" s="29"/>
       <c r="T17" s="29"/>
     </row>
-    <row r="18" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="35"/>
       <c r="B18" s="34" t="s">
         <v>55</v>
@@ -5293,7 +5296,7 @@
       <c r="S18" s="29"/>
       <c r="T18" s="29"/>
     </row>
-    <row r="19" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
       <c r="B19" s="34" t="s">
         <v>54</v>
@@ -5316,7 +5319,7 @@
       <c r="S19" s="29"/>
       <c r="T19" s="29"/>
     </row>
-    <row r="20" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
       <c r="B20" s="34"/>
       <c r="C20" s="33" t="s">
@@ -5339,7 +5342,7 @@
       <c r="S20" s="29"/>
       <c r="T20" s="29"/>
     </row>
-    <row r="21" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" s="34"/>
       <c r="C21" s="33" t="s">
@@ -5362,7 +5365,7 @@
       <c r="S21" s="29"/>
       <c r="T21" s="29"/>
     </row>
-    <row r="22" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="35"/>
       <c r="B22" s="37"/>
       <c r="C22" s="33" t="s">
@@ -5385,7 +5388,7 @@
       <c r="S22" s="29"/>
       <c r="T22" s="29"/>
     </row>
-    <row r="23" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35"/>
       <c r="B23" s="37"/>
       <c r="C23" s="33" t="s">
@@ -5408,7 +5411,7 @@
       <c r="S23" s="29"/>
       <c r="T23" s="29"/>
     </row>
-    <row r="24" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="35"/>
       <c r="B24" s="37"/>
       <c r="C24" s="33" t="s">
@@ -5431,7 +5434,7 @@
       <c r="S24" s="29"/>
       <c r="T24" s="29"/>
     </row>
-    <row r="25" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="35"/>
       <c r="B25" s="34"/>
       <c r="C25" s="33" t="s">
@@ -5454,7 +5457,7 @@
       <c r="S25" s="29"/>
       <c r="T25" s="29"/>
     </row>
-    <row r="26" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="35"/>
       <c r="B26" s="34"/>
       <c r="C26" s="33" t="s">
@@ -5477,7 +5480,7 @@
       <c r="S26" s="29"/>
       <c r="T26" s="29"/>
     </row>
-    <row r="27" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="35"/>
       <c r="B27" s="34" t="s">
         <v>46</v>
@@ -5500,7 +5503,7 @@
       <c r="S27" s="29"/>
       <c r="T27" s="29"/>
     </row>
-    <row r="28" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="35"/>
       <c r="B28" s="34"/>
       <c r="C28" s="33" t="s">
@@ -5523,7 +5526,7 @@
       <c r="S28" s="29"/>
       <c r="T28" s="29"/>
     </row>
-    <row r="29" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="35"/>
       <c r="B29" s="34"/>
       <c r="C29" s="33" t="s">
@@ -5546,7 +5549,7 @@
       <c r="S29" s="29"/>
       <c r="T29" s="29"/>
     </row>
-    <row r="30" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="35"/>
       <c r="B30" s="34"/>
       <c r="C30" s="33" t="s">
@@ -5569,7 +5572,7 @@
       <c r="S30" s="29"/>
       <c r="T30" s="29"/>
     </row>
-    <row r="31" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="35"/>
       <c r="B31" s="34"/>
       <c r="C31" s="33" t="s">
@@ -5592,7 +5595,7 @@
       <c r="S31" s="29"/>
       <c r="T31" s="29"/>
     </row>
-    <row r="32" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="35"/>
       <c r="B32" s="34"/>
       <c r="C32" s="33" t="s">
@@ -5615,7 +5618,7 @@
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
     </row>
-    <row r="33" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="35"/>
       <c r="B33" s="34"/>
       <c r="C33" s="33" t="s">
@@ -5638,7 +5641,7 @@
       <c r="S33" s="29"/>
       <c r="T33" s="29"/>
     </row>
-    <row r="34" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="35"/>
       <c r="B34" s="34" t="s">
         <v>39</v>
@@ -5661,7 +5664,7 @@
       <c r="S34" s="29"/>
       <c r="T34" s="29"/>
     </row>
-    <row r="35" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="35"/>
       <c r="B35" s="34"/>
       <c r="C35" s="33" t="s">
@@ -5684,7 +5687,7 @@
       <c r="S35" s="29"/>
       <c r="T35" s="29"/>
     </row>
-    <row r="36" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="35"/>
       <c r="B36" s="34"/>
       <c r="C36" s="33" t="s">
@@ -5707,7 +5710,7 @@
       <c r="S36" s="29"/>
       <c r="T36" s="29"/>
     </row>
-    <row r="37" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="35"/>
       <c r="B37" s="34"/>
       <c r="C37" s="33" t="s">
@@ -5730,7 +5733,7 @@
       <c r="S37" s="29"/>
       <c r="T37" s="29"/>
     </row>
-    <row r="38" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="35"/>
       <c r="B38" s="34"/>
       <c r="C38" s="33" t="s">
@@ -5753,7 +5756,7 @@
       <c r="S38" s="29"/>
       <c r="T38" s="29"/>
     </row>
-    <row r="39" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="35"/>
       <c r="B39" s="34"/>
       <c r="C39" s="33" t="s">
@@ -5776,7 +5779,7 @@
       <c r="S39" s="29"/>
       <c r="T39" s="29"/>
     </row>
-    <row r="40" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="35"/>
       <c r="B40" s="34"/>
       <c r="C40" s="33" t="s">
@@ -5799,7 +5802,7 @@
       <c r="S40" s="29"/>
       <c r="T40" s="29"/>
     </row>
-    <row r="41" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="35"/>
       <c r="B41" s="34"/>
       <c r="C41" s="33" t="s">
@@ -5822,7 +5825,7 @@
       <c r="S41" s="29"/>
       <c r="T41" s="29"/>
     </row>
-    <row r="42" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="35"/>
       <c r="B42" s="34" t="s">
         <v>31</v>
@@ -5845,7 +5848,7 @@
       <c r="S42" s="29"/>
       <c r="T42" s="29"/>
     </row>
-    <row r="43" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="35"/>
       <c r="B43" s="34"/>
       <c r="C43" s="33" t="s">
@@ -5868,7 +5871,7 @@
       <c r="S43" s="29"/>
       <c r="T43" s="29"/>
     </row>
-    <row r="44" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="35"/>
       <c r="B44" s="34"/>
       <c r="C44" s="33" t="s">
@@ -5891,7 +5894,7 @@
       <c r="S44" s="29"/>
       <c r="T44" s="29"/>
     </row>
-    <row r="45" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35"/>
       <c r="B45" s="34"/>
       <c r="C45" s="33" t="s">
@@ -5914,7 +5917,7 @@
       <c r="S45" s="29"/>
       <c r="T45" s="29"/>
     </row>
-    <row r="46" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="35"/>
       <c r="B46" s="34"/>
       <c r="C46" s="33" t="s">
@@ -5937,7 +5940,7 @@
       <c r="S46" s="29"/>
       <c r="T46" s="29"/>
     </row>
-    <row r="47" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="35"/>
       <c r="B47" s="34"/>
       <c r="C47" s="33" t="s">
@@ -5960,7 +5963,7 @@
       <c r="S47" s="29"/>
       <c r="T47" s="29"/>
     </row>
-    <row r="48" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="35"/>
       <c r="B48" s="34"/>
       <c r="C48" s="33" t="s">
@@ -5983,7 +5986,7 @@
       <c r="S48" s="29"/>
       <c r="T48" s="29"/>
     </row>
-    <row r="49" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" s="25" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A49" s="28"/>
       <c r="B49" s="27"/>
       <c r="C49" s="27"/>
@@ -6018,18 +6021,18 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="19" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" style="19" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.28515625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="43.85546875" style="19" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="19"/>
+    <col min="2" max="2" width="4.88671875" style="19" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.33203125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="43.88671875" style="19" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="159" t="s">
         <v>113</v>
       </c>
@@ -6039,7 +6042,7 @@
       <c r="F3" s="160"/>
       <c r="G3" s="160"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="68"/>
       <c r="B5" s="67"/>
       <c r="C5" s="67"/>
@@ -6059,22 +6062,22 @@
       <c r="F6" s="163"/>
       <c r="G6" s="164"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="52"/>
       <c r="G7" s="51"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
       <c r="B8" s="31" t="s">
         <v>111</v>
       </c>
       <c r="G8" s="51"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
       <c r="G9" s="51"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="52"/>
       <c r="B10" s="50" t="s">
         <v>110</v>
@@ -6085,7 +6088,7 @@
       <c r="F10" s="31"/>
       <c r="G10" s="51"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="52"/>
       <c r="B11" s="31"/>
       <c r="C11" s="48" t="s">
@@ -6096,7 +6099,7 @@
       <c r="F11" s="31"/>
       <c r="G11" s="51"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="52"/>
       <c r="B12" s="31"/>
       <c r="C12" s="48" t="s">
@@ -6107,7 +6110,7 @@
       <c r="F12" s="31"/>
       <c r="G12" s="51"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="52"/>
       <c r="B13" s="31"/>
       <c r="C13" s="48" t="s">
@@ -6118,7 +6121,7 @@
       <c r="F13" s="31"/>
       <c r="G13" s="51"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="52"/>
       <c r="B14" s="31"/>
       <c r="C14" s="48" t="s">
@@ -6129,7 +6132,7 @@
       <c r="F14" s="31"/>
       <c r="G14" s="51"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="52"/>
       <c r="B15" s="31"/>
       <c r="C15" s="48" t="s">
@@ -6140,7 +6143,7 @@
       <c r="F15" s="31"/>
       <c r="G15" s="51"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="52"/>
       <c r="B16" s="31"/>
       <c r="C16" s="48" t="s">
@@ -6151,7 +6154,7 @@
       <c r="F16" s="31"/>
       <c r="G16" s="51"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="52"/>
       <c r="B17" s="31"/>
       <c r="C17" s="48" t="s">
@@ -6162,7 +6165,7 @@
       <c r="F17" s="31"/>
       <c r="G17" s="51"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="45"/>
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
@@ -6171,7 +6174,7 @@
       <c r="F18" s="44"/>
       <c r="G18" s="43"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="68"/>
       <c r="B20" s="67"/>
       <c r="C20" s="67"/>
@@ -6191,22 +6194,22 @@
       <c r="F21" s="163"/>
       <c r="G21" s="164"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="52"/>
       <c r="G22" s="51"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="52"/>
       <c r="B23" s="31" t="s">
         <v>85</v>
       </c>
       <c r="G23" s="51"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="52"/>
       <c r="G24" s="51"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="52"/>
       <c r="B25" s="50" t="s">
         <v>101</v>
@@ -6217,7 +6220,7 @@
       <c r="F25" s="31"/>
       <c r="G25" s="51"/>
     </row>
-    <row r="26" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="52"/>
       <c r="B26" s="31"/>
       <c r="C26" s="166" t="s">
@@ -6228,7 +6231,7 @@
       <c r="F26" s="166"/>
       <c r="G26" s="51"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="52"/>
       <c r="B27" s="31"/>
       <c r="C27" s="48" t="s">
@@ -6239,7 +6242,7 @@
       <c r="F27" s="31"/>
       <c r="G27" s="51"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="52"/>
       <c r="B28" s="31"/>
       <c r="C28" s="48" t="s">
@@ -6250,7 +6253,7 @@
       <c r="F28" s="31"/>
       <c r="G28" s="51"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="45"/>
       <c r="B29" s="44"/>
       <c r="C29" s="44"/>
@@ -6259,7 +6262,7 @@
       <c r="F29" s="44"/>
       <c r="G29" s="43"/>
     </row>
-    <row r="31" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="57"/>
       <c r="B31" s="56"/>
       <c r="C31" s="56"/>
@@ -6279,7 +6282,7 @@
       <c r="F32" s="163"/>
       <c r="G32" s="164"/>
     </row>
-    <row r="33" spans="1:20" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="49"/>
       <c r="G33" s="30"/>
       <c r="I33" s="54"/>
@@ -6295,18 +6298,18 @@
       <c r="S33" s="53"/>
       <c r="T33" s="53"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="52"/>
       <c r="B34" s="31" t="s">
         <v>85</v>
       </c>
       <c r="G34" s="51"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="52"/>
       <c r="G35" s="51"/>
     </row>
-    <row r="36" spans="1:20" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="49"/>
       <c r="B36" s="64" t="s">
         <v>96</v>
@@ -6329,7 +6332,7 @@
       <c r="S36" s="53"/>
       <c r="T36" s="53"/>
     </row>
-    <row r="37" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="49"/>
       <c r="B37" s="64" t="s">
         <v>95</v>
@@ -6348,7 +6351,7 @@
       <c r="S37" s="46"/>
       <c r="T37" s="46"/>
     </row>
-    <row r="38" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="49"/>
       <c r="B38" s="64" t="s">
         <v>94</v>
@@ -6367,7 +6370,7 @@
       <c r="S38" s="46"/>
       <c r="T38" s="46"/>
     </row>
-    <row r="39" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="49"/>
       <c r="B39" s="64" t="s">
         <v>93</v>
@@ -6386,7 +6389,7 @@
       <c r="S39" s="46"/>
       <c r="T39" s="46"/>
     </row>
-    <row r="40" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="49"/>
       <c r="B40" s="64" t="s">
         <v>92</v>
@@ -6406,7 +6409,7 @@
       <c r="S40" s="46"/>
       <c r="T40" s="46"/>
     </row>
-    <row r="41" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="49"/>
       <c r="B41" s="64" t="s">
         <v>91</v>
@@ -6426,7 +6429,7 @@
       <c r="S41" s="46"/>
       <c r="T41" s="46"/>
     </row>
-    <row r="42" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="49"/>
       <c r="B42" s="64" t="s">
         <v>90</v>
@@ -6445,7 +6448,7 @@
       <c r="S42" s="46"/>
       <c r="T42" s="46"/>
     </row>
-    <row r="43" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="49"/>
       <c r="B43" s="64" t="s">
         <v>89</v>
@@ -6464,7 +6467,7 @@
       <c r="S43" s="46"/>
       <c r="T43" s="46"/>
     </row>
-    <row r="44" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="49"/>
       <c r="B44" s="64" t="s">
         <v>88</v>
@@ -6483,7 +6486,7 @@
       <c r="S44" s="46"/>
       <c r="T44" s="46"/>
     </row>
-    <row r="45" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="49"/>
       <c r="B45" s="165" t="s">
         <v>87</v>
@@ -6506,7 +6509,7 @@
       <c r="S45" s="46"/>
       <c r="T45" s="46"/>
     </row>
-    <row r="46" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="62"/>
       <c r="B46" s="61"/>
       <c r="C46" s="61"/>
@@ -6515,7 +6518,7 @@
       <c r="F46" s="61"/>
       <c r="G46" s="60"/>
     </row>
-    <row r="48" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="57"/>
       <c r="B48" s="56"/>
       <c r="C48" s="56"/>
@@ -6535,7 +6538,7 @@
       <c r="F49" s="163"/>
       <c r="G49" s="164"/>
     </row>
-    <row r="50" spans="1:20" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="49"/>
       <c r="G50" s="30"/>
       <c r="I50" s="54"/>
@@ -6551,18 +6554,18 @@
       <c r="S50" s="53"/>
       <c r="T50" s="53"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="52"/>
       <c r="B51" s="31" t="s">
         <v>85</v>
       </c>
       <c r="G51" s="51"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="52"/>
       <c r="G52" s="51"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="52"/>
       <c r="B53" s="50" t="s">
         <v>84</v>
@@ -6572,7 +6575,7 @@
       <c r="E53" s="31"/>
       <c r="G53" s="51"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="52"/>
       <c r="B54" s="58" t="s">
         <v>76</v>
@@ -6584,7 +6587,7 @@
       <c r="E54" s="31"/>
       <c r="G54" s="51"/>
     </row>
-    <row r="55" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="52"/>
       <c r="B55" s="58"/>
       <c r="C55" s="59" t="s">
@@ -6594,7 +6597,7 @@
       <c r="E55" s="36"/>
       <c r="G55" s="51"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="52"/>
       <c r="B56" s="58"/>
       <c r="C56" s="59" t="s">
@@ -6604,7 +6607,7 @@
       <c r="E56" s="36"/>
       <c r="G56" s="51"/>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="52"/>
       <c r="B57" s="58"/>
       <c r="C57" s="59" t="s">
@@ -6614,7 +6617,7 @@
       <c r="E57" s="36"/>
       <c r="G57" s="51"/>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="52"/>
       <c r="B58" s="58"/>
       <c r="C58" s="59" t="s">
@@ -6624,7 +6627,7 @@
       <c r="E58" s="36"/>
       <c r="G58" s="51"/>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="52"/>
       <c r="B59" s="58" t="s">
         <v>76</v>
@@ -6636,7 +6639,7 @@
       <c r="E59" s="36"/>
       <c r="G59" s="51"/>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="52"/>
       <c r="B60" s="58" t="s">
         <v>76</v>
@@ -6648,7 +6651,7 @@
       <c r="E60" s="31"/>
       <c r="G60" s="51"/>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="52"/>
       <c r="B61" s="58" t="s">
         <v>76</v>
@@ -6660,7 +6663,7 @@
       <c r="E61" s="31"/>
       <c r="G61" s="51"/>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="45"/>
       <c r="B62" s="44"/>
       <c r="C62" s="44"/>
@@ -6669,7 +6672,7 @@
       <c r="F62" s="44"/>
       <c r="G62" s="43"/>
     </row>
-    <row r="64" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="57"/>
       <c r="B64" s="56"/>
       <c r="C64" s="56"/>
@@ -6689,7 +6692,7 @@
       <c r="F65" s="163"/>
       <c r="G65" s="164"/>
     </row>
-    <row r="66" spans="1:20" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:20" s="31" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="49"/>
       <c r="G66" s="30"/>
       <c r="I66" s="54"/>
@@ -6705,18 +6708,18 @@
       <c r="S66" s="53"/>
       <c r="T66" s="53"/>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="52"/>
       <c r="B67" s="31" t="s">
         <v>73</v>
       </c>
       <c r="G67" s="51"/>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="52"/>
       <c r="G68" s="51"/>
     </row>
-    <row r="69" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="49"/>
       <c r="B69" s="50" t="s">
         <v>72</v>
@@ -6735,7 +6738,7 @@
       <c r="S69" s="46"/>
       <c r="T69" s="46"/>
     </row>
-    <row r="70" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="49"/>
       <c r="C70" s="48" t="s">
         <v>71</v>
@@ -6754,7 +6757,7 @@
       <c r="S70" s="46"/>
       <c r="T70" s="46"/>
     </row>
-    <row r="71" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="49"/>
       <c r="C71" s="48" t="s">
         <v>70</v>
@@ -6773,7 +6776,7 @@
       <c r="S71" s="46"/>
       <c r="T71" s="46"/>
     </row>
-    <row r="72" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="49"/>
       <c r="B72" s="19"/>
       <c r="C72" s="19"/>
@@ -6792,7 +6795,7 @@
       <c r="S72" s="46"/>
       <c r="T72" s="46"/>
     </row>
-    <row r="73" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="49"/>
       <c r="B73" s="50" t="s">
         <v>69</v>
@@ -6811,7 +6814,7 @@
       <c r="S73" s="46"/>
       <c r="T73" s="46"/>
     </row>
-    <row r="74" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="49"/>
       <c r="C74" s="48" t="s">
         <v>68</v>
@@ -6831,7 +6834,7 @@
       <c r="S74" s="46"/>
       <c r="T74" s="46"/>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="45"/>
       <c r="B75" s="44"/>
       <c r="C75" s="44"/>
@@ -6875,168 +6878,174 @@
       <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" style="25" customWidth="1"/>
-    <col min="2" max="2" width="55.85546875" style="25" customWidth="1"/>
-    <col min="3" max="3" width="64.42578125" style="71" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" style="70" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="71" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="71" hidden="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="25"/>
+    <col min="1" max="1" width="39.6640625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="55.88671875" style="25" customWidth="1"/>
+    <col min="3" max="3" width="64.44140625" style="71" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" style="70" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" style="71" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="71" hidden="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="170" t="s">
+    <row r="1" spans="1:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="181" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
       <c r="D1" s="69"/>
       <c r="E1" s="25"/>
       <c r="F1" s="25"/>
     </row>
-    <row r="4" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="171" t="s">
+    <row r="4" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A4" s="178" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="172"/>
-      <c r="C4" s="173"/>
-    </row>
-    <row r="5" spans="1:6" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="167" t="s">
+      <c r="B4" s="182"/>
+      <c r="C4" s="183"/>
+    </row>
+    <row r="5" spans="1:6" ht="159.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="173" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="168"/>
-      <c r="C5" s="169"/>
-    </row>
-    <row r="6" spans="1:6" ht="205.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="167" t="s">
+      <c r="B5" s="174"/>
+      <c r="C5" s="175"/>
+    </row>
+    <row r="6" spans="1:6" ht="205.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="173" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="168"/>
-      <c r="C6" s="169"/>
-    </row>
-    <row r="9" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="174" t="s">
+      <c r="B6" s="174"/>
+      <c r="C6" s="175"/>
+    </row>
+    <row r="9" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="184" t="s">
         <v>117</v>
       </c>
-      <c r="B9" s="175"/>
-      <c r="C9" s="176"/>
-    </row>
-    <row r="10" spans="1:6" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="167" t="s">
+      <c r="B9" s="179"/>
+      <c r="C9" s="180"/>
+    </row>
+    <row r="10" spans="1:6" ht="115.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="173" t="s">
         <v>118</v>
       </c>
-      <c r="B10" s="168"/>
-      <c r="C10" s="169"/>
-    </row>
-    <row r="11" spans="1:6" ht="192" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="167" t="s">
+      <c r="B10" s="174"/>
+      <c r="C10" s="175"/>
+    </row>
+    <row r="11" spans="1:6" ht="192" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="173" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="168"/>
-      <c r="C11" s="169"/>
-    </row>
-    <row r="12" spans="1:6" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="167" t="s">
+      <c r="B11" s="174"/>
+      <c r="C11" s="175"/>
+    </row>
+    <row r="12" spans="1:6" ht="129.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="173" t="s">
         <v>120</v>
       </c>
-      <c r="B12" s="168"/>
-      <c r="C12" s="169"/>
-    </row>
-    <row r="14" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="183" t="s">
+      <c r="B12" s="174"/>
+      <c r="C12" s="175"/>
+    </row>
+    <row r="14" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="176" t="s">
         <v>121</v>
       </c>
-      <c r="B14" s="184"/>
-      <c r="C14" s="184"/>
-    </row>
-    <row r="15" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="177"/>
+      <c r="C14" s="177"/>
+    </row>
+    <row r="15" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="72"/>
       <c r="C15" s="25"/>
     </row>
-    <row r="17" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A17" s="171" t="s">
+    <row r="17" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A17" s="178" t="s">
         <v>122</v>
       </c>
-      <c r="B17" s="175"/>
-      <c r="C17" s="176"/>
-    </row>
-    <row r="18" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="179"/>
+      <c r="C17" s="180"/>
+    </row>
+    <row r="18" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="73" t="s">
         <v>123</v>
       </c>
       <c r="B18" s="74"/>
       <c r="C18" s="75"/>
     </row>
-    <row r="19" spans="1:6" s="70" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="177" t="s">
+    <row r="19" spans="1:6" s="70" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="167" t="s">
         <v>124</v>
       </c>
-      <c r="B19" s="178"/>
+      <c r="B19" s="168"/>
       <c r="C19" s="76" t="s">
         <v>125</v>
       </c>
       <c r="E19" s="71"/>
       <c r="F19" s="71"/>
     </row>
-    <row r="20" spans="1:6" s="70" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="177" t="s">
+    <row r="20" spans="1:6" s="70" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="167" t="s">
         <v>126</v>
       </c>
-      <c r="B20" s="178"/>
+      <c r="B20" s="168"/>
       <c r="C20" s="76" t="s">
         <v>125</v>
       </c>
       <c r="E20" s="71"/>
       <c r="F20" s="71"/>
     </row>
-    <row r="21" spans="1:6" s="70" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="177" t="s">
+    <row r="21" spans="1:6" s="70" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="167" t="s">
         <v>127</v>
       </c>
-      <c r="B21" s="178"/>
+      <c r="B21" s="168"/>
       <c r="C21" s="76" t="s">
         <v>128</v>
       </c>
       <c r="E21" s="71"/>
       <c r="F21" s="71"/>
     </row>
-    <row r="22" spans="1:6" s="70" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="70" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="77"/>
       <c r="B22" s="78"/>
       <c r="C22" s="76"/>
       <c r="E22" s="71"/>
       <c r="F22" s="71"/>
     </row>
-    <row r="23" spans="1:6" s="70" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="177" t="s">
+    <row r="23" spans="1:6" s="70" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="167" t="s">
         <v>129</v>
       </c>
-      <c r="B23" s="178"/>
-      <c r="C23" s="179"/>
+      <c r="B23" s="168"/>
+      <c r="C23" s="169"/>
       <c r="E23" s="71"/>
       <c r="F23" s="71"/>
     </row>
-    <row r="24" spans="1:6" s="70" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" s="70" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="77"/>
       <c r="B24" s="78"/>
       <c r="C24" s="76"/>
       <c r="E24" s="71"/>
       <c r="F24" s="71"/>
     </row>
-    <row r="25" spans="1:6" s="70" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="180" t="s">
+    <row r="25" spans="1:6" s="70" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="170" t="s">
         <v>130</v>
       </c>
-      <c r="B25" s="181"/>
-      <c r="C25" s="182"/>
+      <c r="B25" s="171"/>
+      <c r="C25" s="172"/>
       <c r="E25" s="71"/>
       <c r="F25" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A9:C9"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A25:C25"/>
@@ -7046,12 +7055,6 @@
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -7073,16 +7076,16 @@
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="1.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="1.42578125" customWidth="1"/>
+    <col min="5" max="5" width="1.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="80"/>
       <c r="B1" s="81" t="s">
         <v>131</v>
@@ -7095,7 +7098,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="80"/>
       <c r="B2" s="83" t="s">
         <v>146</v>
@@ -7110,7 +7113,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="80"/>
       <c r="B3" s="83" t="s">
         <v>146</v>
@@ -7125,7 +7128,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="80"/>
       <c r="B4" s="84" t="s">
         <v>132</v>
@@ -7136,7 +7139,7 @@
       <c r="D4" s="85"/>
       <c r="E4" s="80"/>
     </row>
-    <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="80"/>
       <c r="B5" s="85"/>
       <c r="C5" s="85" t="s">
@@ -7145,7 +7148,7 @@
       <c r="D5" s="85"/>
       <c r="E5" s="80"/>
     </row>
-    <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="80"/>
       <c r="B6" s="85"/>
       <c r="C6" s="85" t="s">
@@ -7154,21 +7157,21 @@
       <c r="D6" s="85"/>
       <c r="E6" s="80"/>
     </row>
-    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="80"/>
       <c r="B7" s="85"/>
       <c r="C7" s="85"/>
       <c r="D7" s="85"/>
       <c r="E7" s="80"/>
     </row>
-    <row r="8" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="86"/>
       <c r="B8" s="87"/>
       <c r="C8" s="87"/>
       <c r="D8" s="88"/>
       <c r="E8" s="80"/>
     </row>
-    <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="89"/>
       <c r="B9" s="84" t="s">
         <v>136</v>
@@ -7177,14 +7180,14 @@
       <c r="D9" s="90"/>
       <c r="E9" s="80"/>
     </row>
-    <row r="10" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="89"/>
       <c r="B10" s="84"/>
       <c r="C10" s="85"/>
       <c r="D10" s="90"/>
       <c r="E10" s="80"/>
     </row>
-    <row r="11" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="89"/>
       <c r="B11" s="85" t="s">
         <v>137</v>
@@ -7195,7 +7198,7 @@
       <c r="D11" s="91"/>
       <c r="E11" s="80"/>
     </row>
-    <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="89"/>
       <c r="B12" s="85" t="s">
         <v>138</v>
@@ -7207,7 +7210,7 @@
       <c r="D12" s="91"/>
       <c r="E12" s="80"/>
     </row>
-    <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="89"/>
       <c r="B13" s="85" t="s">
         <v>139</v>
@@ -7218,7 +7221,7 @@
       <c r="D13" s="91"/>
       <c r="E13" s="80"/>
     </row>
-    <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="89"/>
       <c r="B14" s="85" t="s">
         <v>140</v>
@@ -7229,7 +7232,7 @@
       <c r="D14" s="91"/>
       <c r="E14" s="80"/>
     </row>
-    <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="89"/>
       <c r="B15" s="85"/>
       <c r="C15" s="97">
@@ -7239,21 +7242,21 @@
       <c r="D15" s="90"/>
       <c r="E15" s="80"/>
     </row>
-    <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="89"/>
       <c r="B16" s="85"/>
       <c r="C16" s="85"/>
       <c r="D16" s="90"/>
       <c r="E16" s="80"/>
     </row>
-    <row r="17" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="89"/>
       <c r="B17" s="85"/>
       <c r="C17" s="85"/>
       <c r="D17" s="90"/>
       <c r="E17" s="80"/>
     </row>
-    <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="89"/>
       <c r="B18" s="84" t="s">
         <v>141</v>
@@ -7262,14 +7265,14 @@
       <c r="D18" s="90"/>
       <c r="E18" s="80"/>
     </row>
-    <row r="19" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="89"/>
       <c r="B19" s="84"/>
       <c r="C19" s="85"/>
       <c r="D19" s="90"/>
       <c r="E19" s="80"/>
     </row>
-    <row r="20" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="89"/>
       <c r="B20" s="85" t="s">
         <v>142</v>
@@ -7280,7 +7283,7 @@
       <c r="D20" s="91"/>
       <c r="E20" s="80"/>
     </row>
-    <row r="21" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="89"/>
       <c r="B21" s="85" t="s">
         <v>139</v>
@@ -7291,7 +7294,7 @@
       <c r="D21" s="91"/>
       <c r="E21" s="80"/>
     </row>
-    <row r="22" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="89"/>
       <c r="B22" s="85" t="s">
         <v>140</v>
@@ -7302,7 +7305,7 @@
       <c r="D22" s="91"/>
       <c r="E22" s="80"/>
     </row>
-    <row r="23" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="89"/>
       <c r="B23" s="85"/>
       <c r="C23" s="97">
@@ -7312,21 +7315,21 @@
       <c r="D23" s="90"/>
       <c r="E23" s="80"/>
     </row>
-    <row r="24" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="89"/>
       <c r="B24" s="85"/>
       <c r="C24" s="85"/>
       <c r="D24" s="90"/>
       <c r="E24" s="80"/>
     </row>
-    <row r="25" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="89"/>
       <c r="B25" s="85"/>
       <c r="C25" s="85"/>
       <c r="D25" s="90"/>
       <c r="E25" s="80"/>
     </row>
-    <row r="26" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="89"/>
       <c r="B26" s="84" t="s">
         <v>143</v>
@@ -7335,14 +7338,14 @@
       <c r="D26" s="90"/>
       <c r="E26" s="80"/>
     </row>
-    <row r="27" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="89"/>
       <c r="B27" s="84"/>
       <c r="C27" s="85"/>
       <c r="D27" s="90"/>
       <c r="E27" s="80"/>
     </row>
-    <row r="28" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="89"/>
       <c r="B28" s="92" t="s">
         <v>144</v>
@@ -7353,7 +7356,7 @@
       <c r="D28" s="90"/>
       <c r="E28" s="80"/>
     </row>
-    <row r="29" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="89"/>
       <c r="B29" s="98">
         <v>1</v>
@@ -7365,7 +7368,7 @@
       <c r="D29" s="90"/>
       <c r="E29" s="80"/>
     </row>
-    <row r="30" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="89"/>
       <c r="B30" s="98">
         <v>2</v>
@@ -7377,7 +7380,7 @@
       <c r="D30" s="90"/>
       <c r="E30" s="80"/>
     </row>
-    <row r="31" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="89"/>
       <c r="B31" s="98">
         <v>3</v>
@@ -7389,7 +7392,7 @@
       <c r="D31" s="90"/>
       <c r="E31" s="80"/>
     </row>
-    <row r="32" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="89"/>
       <c r="B32" s="98">
         <v>4</v>
@@ -7401,7 +7404,7 @@
       <c r="D32" s="90"/>
       <c r="E32" s="80"/>
     </row>
-    <row r="33" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="89"/>
       <c r="B33" s="98">
         <v>5</v>
@@ -7413,63 +7416,63 @@
       <c r="D33" s="90"/>
       <c r="E33" s="80"/>
     </row>
-    <row r="34" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="93"/>
       <c r="B34" s="94"/>
       <c r="C34" s="94"/>
       <c r="D34" s="95"/>
       <c r="E34" s="80"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="80"/>
       <c r="B35" s="80"/>
       <c r="C35" s="80"/>
       <c r="D35" s="80"/>
       <c r="E35" s="80"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="80"/>
       <c r="B36" s="80"/>
       <c r="C36" s="80"/>
       <c r="D36" s="80"/>
       <c r="E36" s="80"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="80"/>
       <c r="B37" s="80"/>
       <c r="C37" s="80"/>
       <c r="D37" s="80"/>
       <c r="E37" s="80"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="79"/>
       <c r="B38" s="79"/>
       <c r="C38" s="79"/>
       <c r="D38" s="79"/>
       <c r="E38" s="79"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="79"/>
       <c r="B39" s="79"/>
       <c r="C39" s="79"/>
       <c r="D39" s="79"/>
       <c r="E39" s="79"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="79"/>
       <c r="B40" s="79"/>
       <c r="C40" s="79"/>
       <c r="D40" s="79"/>
       <c r="E40" s="79"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="79"/>
       <c r="B41" s="79"/>
       <c r="C41" s="79"/>
       <c r="D41" s="79"/>
       <c r="E41" s="79"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="79"/>
       <c r="B42" s="79"/>
       <c r="C42" s="79"/>
@@ -7491,28 +7494,28 @@
   </sheetPr>
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.7109375" style="72" customWidth="1"/>
-    <col min="2" max="2" width="53.28515625" style="25" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="25"/>
+    <col min="1" max="1" width="52.6640625" style="72" customWidth="1"/>
+    <col min="2" max="2" width="53.33203125" style="25" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="189" t="s">
+    <row r="1" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="186" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="189"/>
-    </row>
-    <row r="2" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="190"/>
-      <c r="B2" s="190"/>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="186"/>
+    </row>
+    <row r="2" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="187"/>
+      <c r="B2" s="187"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="117" t="s">
         <v>188</v>
       </c>
@@ -7520,23 +7523,23 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="114"/>
       <c r="B4" s="65"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="115" t="s">
         <v>186</v>
       </c>
       <c r="B5" s="63"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="114" t="s">
         <v>185</v>
       </c>
       <c r="B6" s="65"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="114" t="s">
         <v>184</v>
       </c>
@@ -7544,7 +7547,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="114" t="s">
         <v>182</v>
       </c>
@@ -7552,7 +7555,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="114" t="s">
         <v>180</v>
       </c>
@@ -7560,26 +7563,26 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="112" t="s">
         <v>178</v>
       </c>
       <c r="B10" s="65"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="111"/>
       <c r="B11" s="110"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12" s="72"/>
     </row>
-    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="106" t="s">
         <v>177</v>
       </c>
       <c r="B13" s="105"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="102" t="s">
         <v>176</v>
       </c>
@@ -7587,7 +7590,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="102" t="s">
         <v>174</v>
       </c>
@@ -7595,7 +7598,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="102" t="s">
         <v>172</v>
       </c>
@@ -7603,194 +7606,187 @@
         <v>171</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="103"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="106" t="s">
         <v>170</v>
       </c>
       <c r="B18" s="105"/>
     </row>
-    <row r="19" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="165" t="s">
         <v>169</v>
       </c>
       <c r="B19" s="165"/>
     </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="103"/>
       <c r="B20" s="103"/>
     </row>
-    <row r="21" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="106" t="s">
         <v>168</v>
       </c>
       <c r="B21" s="109"/>
     </row>
-    <row r="22" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="165" t="s">
         <v>167</v>
       </c>
       <c r="B22" s="165"/>
     </row>
-    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="106" t="s">
         <v>166</v>
       </c>
       <c r="B24" s="105"/>
     </row>
-    <row r="25" spans="1:8" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="165" t="s">
         <v>165</v>
       </c>
       <c r="B25" s="165"/>
       <c r="D25" s="104"/>
     </row>
-    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="108"/>
       <c r="B26" s="103"/>
     </row>
-    <row r="27" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="106" t="s">
         <v>164</v>
       </c>
       <c r="B27" s="107"/>
     </row>
-    <row r="28" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="165" t="s">
         <v>163</v>
       </c>
       <c r="B28" s="165"/>
-      <c r="D28" s="188"/>
-      <c r="E28" s="188"/>
-      <c r="F28" s="188"/>
-      <c r="G28" s="188"/>
-      <c r="H28" s="188"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="185"/>
-      <c r="B29" s="185"/>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D28" s="185"/>
+      <c r="E28" s="185"/>
+      <c r="F28" s="185"/>
+      <c r="G28" s="185"/>
+      <c r="H28" s="185"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="188"/>
+      <c r="B29" s="188"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="106" t="s">
         <v>162</v>
       </c>
       <c r="B30" s="107"/>
     </row>
-    <row r="31" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="165" t="s">
         <v>161</v>
       </c>
       <c r="B31" s="165"/>
       <c r="D31" s="104"/>
     </row>
-    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="103"/>
       <c r="B32" s="103"/>
     </row>
-    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="186" t="s">
+    <row r="33" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="189" t="s">
         <v>160</v>
       </c>
-      <c r="B33" s="186"/>
-    </row>
-    <row r="34" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="189"/>
+    </row>
+    <row r="34" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="165" t="s">
         <v>159</v>
       </c>
       <c r="B34" s="165"/>
       <c r="D34" s="104"/>
     </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="106" t="s">
         <v>158</v>
       </c>
       <c r="B36" s="105"/>
     </row>
-    <row r="37" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="165" t="s">
         <v>157</v>
       </c>
       <c r="B37" s="165"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="106" t="s">
         <v>156</v>
       </c>
       <c r="B39" s="105"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="102" t="s">
         <v>155</v>
       </c>
       <c r="B40" s="31"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="102" t="s">
         <v>154</v>
       </c>
       <c r="B41" s="31"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="102" t="s">
         <v>153</v>
       </c>
       <c r="B42" s="31"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="102" t="s">
         <v>152</v>
       </c>
       <c r="B43" s="31"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="47"/>
       <c r="B44" s="31"/>
     </row>
-    <row r="45" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="187" t="s">
+    <row r="45" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="190" t="s">
         <v>151</v>
       </c>
-      <c r="B45" s="187"/>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="190"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="106" t="s">
         <v>150</v>
       </c>
       <c r="B47" s="105"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="102" t="s">
         <v>149</v>
       </c>
       <c r="B48" s="31"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="165" t="s">
         <v>148</v>
       </c>
       <c r="B49" s="165"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="165" t="s">
         <v>147</v>
       </c>
       <c r="B50" s="165"/>
       <c r="D50" s="104"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A28:B28"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="A29:B29"/>
@@ -7799,6 +7795,13 @@
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -7820,16 +7823,16 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" style="131" customWidth="1"/>
     <col min="2" max="2" width="27" style="132" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" style="25" customWidth="1"/>
-    <col min="4" max="4" width="45.5703125" style="25" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="25"/>
+    <col min="3" max="3" width="36.5546875" style="25" customWidth="1"/>
+    <col min="4" max="4" width="45.5546875" style="25" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="118" t="s">
         <v>190</v>
       </c>
@@ -7837,11 +7840,11 @@
       <c r="C1" s="119"/>
       <c r="D1" s="119"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="102"/>
       <c r="B2" s="102"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="120" t="s">
         <v>191</v>
       </c>
@@ -7855,7 +7858,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A4" s="122" t="s">
         <v>195</v>
       </c>
@@ -7869,7 +7872,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A5" s="125" t="s">
         <v>199</v>
       </c>
@@ -7883,7 +7886,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="125" t="s">
         <v>203</v>
       </c>
@@ -7897,7 +7900,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A7" s="125" t="s">
         <v>207</v>
       </c>
@@ -7911,7 +7914,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="125" t="s">
         <v>211</v>
       </c>
@@ -7925,7 +7928,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="125" t="s">
         <v>215</v>
       </c>
@@ -7939,7 +7942,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="125" t="s">
         <v>218</v>
       </c>
@@ -7953,7 +7956,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="125" t="s">
         <v>221</v>
       </c>
@@ -7967,7 +7970,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A12" s="125" t="s">
         <v>224</v>
       </c>

</xml_diff>